<commit_message>
Benchmark reports moved to server/logs/benchmark more benchmarks
</commit_message>
<xml_diff>
--- a/Algos.xlsx
+++ b/Algos.xlsx
@@ -10,12 +10,15 @@
     <sheet name="MSH" sheetId="1" r:id="rId1"/>
     <sheet name="wiki" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MSH!$A$2:$F$2</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="28">
   <si>
     <t>AlgoID</t>
   </si>
@@ -72,13 +75,40 @@
   </si>
   <si>
     <t>v2_small</t>
+  </si>
+  <si>
+    <t>LDA_cossim</t>
+  </si>
+  <si>
+    <t>Doesn't matter, isn't used</t>
+  </si>
+  <si>
+    <t>fromText + LDA_multiclass</t>
+  </si>
+  <si>
+    <t>LDA_multiclass</t>
+  </si>
+  <si>
+    <t>Old Value, needs to be re-computed</t>
+  </si>
+  <si>
+    <t>lda_type1 (no stemming, 2 passes for training LDA)</t>
+  </si>
+  <si>
+    <t>lda_type2 (no stemming, 5 passes for training LDA)</t>
+  </si>
+  <si>
+    <t>lda_type3 (no stemming, removing numbers and "%+=", 3 passes for training LDA)</t>
+  </si>
+  <si>
+    <t>lda_type4 (stemming, removing numbers and "%+=", 3 passes for training LDA)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,13 +116,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,16 +146,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,263 +461,463 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.08984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="78" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="59.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>0.80906800000000001</v>
+      </c>
+      <c r="C3">
+        <v>1.1044E-2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0.78825500000000004</v>
+      </c>
+      <c r="C4">
+        <v>1.1328E-2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0.76947299999999996</v>
+      </c>
+      <c r="C5">
+        <v>1.0144E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0.76762699999999995</v>
+      </c>
+      <c r="C6">
+        <v>1.2021E-2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.75835900000000001</v>
+      </c>
+      <c r="C7">
+        <v>1.4669E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0.75348700000000002</v>
+      </c>
+      <c r="C8">
+        <v>8.3639999999999999E-3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>0.75083100000000003</v>
+      </c>
+      <c r="C9">
+        <v>1.0872E-2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>0.74939500000000003</v>
+      </c>
+      <c r="C10">
+        <v>8.8679999999999991E-3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0.74696700000000005</v>
+      </c>
+      <c r="C11">
+        <v>9.8849999999999997E-3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="B12">
+        <v>0.74454399999999998</v>
+      </c>
+      <c r="C12">
+        <v>1.1891000000000001E-2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>0.734595</v>
+      </c>
+      <c r="C13">
+        <v>9.1070000000000005E-3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.73348199999999997</v>
+      </c>
+      <c r="C14">
+        <v>1.2735E-2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.71223800000000004</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.2111E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B16" s="2">
+        <v>0.64232400000000001</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.1989E-2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B17" s="2">
+        <v>0.63768899999999995</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.0935E-2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.61285800000000001</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.2086E-2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B19" s="2">
         <v>0.59422299999999995</v>
       </c>
-      <c r="C2">
-        <f>0.043496/2</f>
+      <c r="C19" s="2">
         <v>2.1748E-2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D19" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B20" s="2">
         <v>0.57452999999999999</v>
       </c>
-      <c r="C3">
-        <f>0.038942/2</f>
+      <c r="C20" s="2">
         <v>1.9470999999999999E-2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0.61285800000000001</v>
-      </c>
-      <c r="C4">
-        <v>1.2086E-2</v>
-      </c>
-      <c r="D4">
-        <v>0.41742200000000002</v>
-      </c>
-      <c r="E4">
-        <f>0.030252/2</f>
-        <v>1.5126000000000001E-2</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B21" s="2">
+        <v>0.55483800000000005</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2.2133E-2</v>
+      </c>
+      <c r="D21" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>0.55483800000000005</v>
-      </c>
-      <c r="C5">
-        <v>2.2133E-2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>0.64232400000000001</v>
-      </c>
-      <c r="C6">
-        <v>1.1989E-2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>0.63768899999999995</v>
-      </c>
-      <c r="C7">
-        <v>1.0935E-2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>0.71223800000000004</v>
-      </c>
-      <c r="C8">
-        <v>1.2111E-2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>0.70952099999999996</v>
-      </c>
-      <c r="C9">
-        <v>1.3153E-2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>0.80964599999999998</v>
-      </c>
-      <c r="C10">
-        <v>7.8300000000000002E-3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>0.76543600000000001</v>
-      </c>
-      <c r="C11">
-        <v>1.2826000000000001E-2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" t="s">
-        <v>12</v>
+      <c r="E21" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:F2">
+    <sortState ref="A3:F21">
+      <sortCondition descending="1" ref="B2"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Acronyms moved to upper case. (to be undone) Acronym Extractor v3 added, supports acronyms with some smallcase chars new benchmark with extractor v3 failure analysis on algo 18
</commit_message>
<xml_diff>
--- a/Algos.xlsx
+++ b/Algos.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MSH" sheetId="1" r:id="rId1"/>
-    <sheet name="wiki" sheetId="2" r:id="rId2"/>
+    <sheet name="error analysis(temp)" sheetId="3" r:id="rId2"/>
+    <sheet name="wiki" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MSH!$A$2:$F$2</definedName>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="69">
   <si>
     <t>AlgoID</t>
   </si>
@@ -102,6 +103,129 @@
   </si>
   <si>
     <t>lda_type4 (stemming, removing numbers and "%+=", 3 passes for training LDA)</t>
+  </si>
+  <si>
+    <t>v3_small</t>
+  </si>
+  <si>
+    <t>all acronyms stored in uppercase</t>
+  </si>
+  <si>
+    <t>TMP</t>
+  </si>
+  <si>
+    <t>CCL4</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>PCP</t>
+  </si>
+  <si>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>CAM</t>
+  </si>
+  <si>
+    <t>EPI</t>
+  </si>
+  <si>
+    <t>CCD</t>
+  </si>
+  <si>
+    <t>TAT</t>
+  </si>
+  <si>
+    <t>TEM</t>
+  </si>
+  <si>
+    <t>NBS</t>
+  </si>
+  <si>
+    <t>FAS</t>
+  </si>
+  <si>
+    <t>DAT</t>
+  </si>
+  <si>
+    <t>DDS</t>
+  </si>
+  <si>
+    <t>MBP</t>
+  </si>
+  <si>
+    <t>BSA</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>TNT</t>
+  </si>
+  <si>
+    <t>TPA</t>
+  </si>
+  <si>
+    <t>TPO</t>
+  </si>
+  <si>
+    <t>ICE</t>
+  </si>
+  <si>
+    <t>BLM</t>
+  </si>
+  <si>
+    <t>TNC</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>ADH</t>
+  </si>
+  <si>
+    <t>CDA</t>
+  </si>
+  <si>
+    <t>MCC</t>
+  </si>
+  <si>
+    <t>ALA</t>
+  </si>
+  <si>
+    <t>CDR</t>
+  </si>
+  <si>
+    <t>MAF</t>
+  </si>
+  <si>
+    <t>ORF</t>
+  </si>
+  <si>
+    <t>Acronym</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>not detected as acronym</t>
+  </si>
+  <si>
+    <t>case 1Capital, none</t>
+  </si>
+  <si>
+    <t>case none capital</t>
+  </si>
+  <si>
+    <t>1 capital case</t>
   </si>
 </sst>
 </file>
@@ -461,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -912,6 +1036,40 @@
         <v>21</v>
       </c>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>0.90920000000000001</v>
+      </c>
+      <c r="C22">
+        <v>7.6620000000000004E-3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:F2">
     <sortState ref="A3:F21">
@@ -924,6 +1082,387 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="A2:C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="21.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>198</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>159</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>

</xml_diff>